<commit_message>
Write feature descriptions to metadata file
</commit_message>
<xml_diff>
--- a/streamlit_app/Data/metadata/OPERA-models-2.9.xlsx
+++ b/streamlit_app/Data/metadata/OPERA-models-2.9.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkvasnicka\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Repositories\LCIA-QSAR-Model\streamlit_app\data\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3EBC11D-A0EE-4296-AC15-5E294DA40FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C3570A-46B9-450B-961E-816B76FF836E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -399,13 +399,13 @@
     <t>Description</t>
   </si>
   <si>
+    <t>OPERA_Version</t>
+  </si>
+  <si>
+    <t>JRC_Report_ID</t>
+  </si>
+  <si>
     <t>Feature_Name</t>
-  </si>
-  <si>
-    <t>OPERA_Version</t>
-  </si>
-  <si>
-    <t>JRC_Report_ID</t>
   </si>
 </sst>
 </file>
@@ -764,7 +764,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -781,7 +783,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C1" t="s">
         <v>123</v>
@@ -790,13 +792,13 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F1" t="s">
         <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Clean OPERA models Excel file
</commit_message>
<xml_diff>
--- a/streamlit_app/Data/metadata/OPERA-models-2.9.xlsx
+++ b/streamlit_app/Data/metadata/OPERA-models-2.9.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Repositories\LCIA-QSAR-Model\streamlit_app\data\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C3570A-46B9-450B-961E-816B76FF836E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FA973F-90C0-4B5B-9EB0-5122932645BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -114,21 +114,9 @@
     <t>Fish bioconcentration factor</t>
   </si>
   <si>
-    <t xml:space="preserve">biodegradation half-life for compounds containing only carbon and hydrogen </t>
-  </si>
-  <si>
     <t>Ready biodegradability of organic chemicals</t>
   </si>
   <si>
-    <t>Binary 0/1</t>
-  </si>
-  <si>
-    <t>The whole body primary biotransformation rate (half-life) constant for organic chemicals in fish.</t>
-  </si>
-  <si>
-    <t>soil adsorption coefficient of organic compounds.</t>
-  </si>
-  <si>
     <t>QMRF</t>
   </si>
   <si>
@@ -138,21 +126,9 @@
     <t>Melting Point</t>
   </si>
   <si>
-    <t>Degree C</t>
-  </si>
-  <si>
     <t>Vapor Pressure</t>
   </si>
   <si>
-    <t>Water solubility at 25C.</t>
-  </si>
-  <si>
-    <t>Henry’s Law constant (air/water partition coefficient) at 25C</t>
-  </si>
-  <si>
-    <t>The octanol/air partition coefficient.</t>
-  </si>
-  <si>
     <t>count</t>
   </si>
   <si>
@@ -192,21 +168,6 @@
     <t>Collaborative Modeling Project for Androgen Receptor. Antagonist consensus</t>
   </si>
   <si>
-    <t>Binary 0/2</t>
-  </si>
-  <si>
-    <t>Binary 0/3</t>
-  </si>
-  <si>
-    <t>Binary 0/4</t>
-  </si>
-  <si>
-    <t>Binary 0/5</t>
-  </si>
-  <si>
-    <t>Binary 0/6</t>
-  </si>
-  <si>
     <t>Collaborative Acute Toxicity Modeling Suite. LD50 point estimate model</t>
   </si>
   <si>
@@ -406,6 +367,45 @@
   </si>
   <si>
     <t>Feature_Name</t>
+  </si>
+  <si>
+    <t>degree C</t>
+  </si>
+  <si>
+    <t>binary (0/1)</t>
+  </si>
+  <si>
+    <t>binary (0/2)</t>
+  </si>
+  <si>
+    <t>binary (0/3)</t>
+  </si>
+  <si>
+    <t>binary (0/4)</t>
+  </si>
+  <si>
+    <t>binary (0/5)</t>
+  </si>
+  <si>
+    <t>binary (0/6)</t>
+  </si>
+  <si>
+    <t>Octanol-air partition coefficient</t>
+  </si>
+  <si>
+    <t>Henry’s Law constant (air/water partition coefficient) at 25 C</t>
+  </si>
+  <si>
+    <t>Water solubility at 25 C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biodegradation half-life for compounds containing only carbon and hydrogen </t>
+  </si>
+  <si>
+    <t>The whole body primary biotransformation rate (half-life) constant for organic chemicals in fish</t>
+  </si>
+  <si>
+    <t>Soil adsorption coefficient of organic compounds</t>
   </si>
 </sst>
 </file>
@@ -765,7 +765,7 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,22 +783,22 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="C1" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="F1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G1" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -812,7 +812,7 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E2" s="1">
         <v>2.5</v>
@@ -820,13 +820,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E3" s="1">
         <v>2.5</v>
@@ -834,13 +834,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E4" s="1">
         <v>2.5</v>
@@ -848,13 +848,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E5" s="1">
         <v>2.5</v>
@@ -862,13 +862,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E6" s="1">
         <v>2.5</v>
@@ -876,13 +876,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E7" s="1">
         <v>2.5</v>
@@ -890,13 +890,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E8" s="1">
         <v>2.5</v>
@@ -904,13 +904,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="C9" t="s">
         <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E9" s="1">
         <v>2.5</v>
@@ -918,13 +918,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E10" s="1">
         <v>2.5</v>
@@ -938,7 +938,7 @@
         <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E11" s="1">
         <v>2.5</v>
@@ -946,13 +946,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="C12" t="s">
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E12" s="1">
         <v>2.5</v>
@@ -960,13 +960,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="C13" t="s">
         <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E13" s="1">
         <v>2.5</v>
@@ -974,13 +974,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C14" t="s">
         <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E14" s="1">
         <v>2.5</v>
@@ -988,13 +988,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="C15" t="s">
         <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E15" s="1">
         <v>2.5</v>
@@ -1008,7 +1008,7 @@
         <v>23</v>
       </c>
       <c r="D16" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="E16" s="1">
         <v>2.5</v>
@@ -1022,7 +1022,7 @@
         <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="E17" s="1">
         <v>2.5</v>
@@ -1036,7 +1036,7 @@
         <v>25</v>
       </c>
       <c r="D18" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E18" s="1">
         <v>2.5</v>
@@ -1047,122 +1047,122 @@
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>122</v>
       </c>
       <c r="D19" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="E19" s="1">
         <v>2.9</v>
       </c>
       <c r="F19" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="G19" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C20" t="s">
-        <v>41</v>
+        <v>121</v>
       </c>
       <c r="D20" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E20" s="1">
         <v>2.6</v>
       </c>
       <c r="F20" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="G20" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="C21" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D21" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E21" s="1">
         <v>2.9</v>
       </c>
       <c r="F21" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="G21" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="C22" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D22" t="s">
-        <v>37</v>
+        <v>114</v>
       </c>
       <c r="E22" s="1">
         <v>2.9</v>
       </c>
       <c r="F22" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="G22" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D23" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="E23" s="1">
         <v>2.9</v>
       </c>
       <c r="F23" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="G23" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>123</v>
       </c>
       <c r="D24" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="E24" s="1">
         <v>2.9</v>
       </c>
       <c r="F24" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="G24" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1170,138 +1170,138 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="C25" t="s">
         <v>28</v>
       </c>
       <c r="D25" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E25" s="1">
         <v>2.6</v>
       </c>
       <c r="F25" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="G25" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="C26" t="s">
         <v>27</v>
       </c>
       <c r="D26" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="E26" s="1">
         <v>2.6</v>
       </c>
       <c r="F26" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="G26" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="C27" t="s">
-        <v>29</v>
+        <v>124</v>
       </c>
       <c r="D27" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="E27" s="1">
         <v>2.6</v>
       </c>
       <c r="F27" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="G27" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="C28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D28" t="s">
-        <v>31</v>
+        <v>115</v>
       </c>
       <c r="E28" s="1">
         <v>2.6</v>
       </c>
       <c r="F28" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="G28" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>32</v>
+        <v>125</v>
       </c>
       <c r="D29" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="E29" s="1">
         <v>2.6</v>
       </c>
       <c r="F29" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="G29" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>33</v>
+        <v>126</v>
       </c>
       <c r="D30" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="E30" s="1">
         <v>2.6</v>
       </c>
       <c r="F30" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="G30" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D31" t="s">
-        <v>31</v>
+        <v>115</v>
       </c>
       <c r="E31" s="1">
         <v>2.6</v>
@@ -1310,13 +1310,13 @@
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D32" t="s">
-        <v>55</v>
+        <v>116</v>
       </c>
       <c r="E32" s="1">
         <v>2.6</v>
@@ -1325,13 +1325,13 @@
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D33" t="s">
-        <v>56</v>
+        <v>117</v>
       </c>
       <c r="E33" s="1">
         <v>2.6</v>
@@ -1340,13 +1340,13 @@
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D34" t="s">
-        <v>57</v>
+        <v>118</v>
       </c>
       <c r="E34" s="1">
         <v>2.6</v>
@@ -1355,13 +1355,13 @@
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D35" t="s">
-        <v>58</v>
+        <v>119</v>
       </c>
       <c r="E35" s="1">
         <v>2.6</v>
@@ -1370,13 +1370,13 @@
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D36" t="s">
-        <v>59</v>
+        <v>120</v>
       </c>
       <c r="E36" s="1">
         <v>2.6</v>
@@ -1385,13 +1385,13 @@
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="D37" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="E37" s="1">
         <v>2.6</v>
@@ -1400,13 +1400,13 @@
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D38" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="E38" s="1">
         <v>2.8</v>
@@ -1414,16 +1414,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B39" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="C39" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="D39" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="E39" s="1">
         <v>2.8</v>
@@ -1431,13 +1431,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="C40" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="D40" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="E40" s="1">
         <v>2.8</v>

</xml_diff>